<commit_message>
update Test of cases with Gherkin
</commit_message>
<xml_diff>
--- a/DesigandExecution/1.1 Test of cases.xlsx
+++ b/DesigandExecution/1.1 Test of cases.xlsx
@@ -1,19 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadia\Documents\Academy\QAproyect\PetStore\DesigandExecution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F174665F-E70F-4580-96A2-74AB3B7E1D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528F0B7F-4878-451B-BEE6-19B7234A1208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
+    <sheet name="UploadImage" sheetId="1" r:id="rId1"/>
+    <sheet name="FilterPetStatus" sheetId="5" r:id="rId2"/>
+    <sheet name="FilterPetId" sheetId="6" r:id="rId3"/>
+    <sheet name="AggPet" sheetId="2" r:id="rId4"/>
+    <sheet name="UpdatePet" sheetId="3" r:id="rId5"/>
+    <sheet name="UpdateFormPet" sheetId="4" r:id="rId6"/>
+    <sheet name="DeletePet" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="188">
   <si>
     <t>Identificador</t>
   </si>
@@ -183,21 +189,6 @@
 </t>
   </si>
   <si>
-    <t>1. Se debe mostrar status code 201.
-{
-  "id": 0,
-  "category": "perro",
-  "id_category": "1"
-  "name_category": " "
-  "name_mascota:": "Loli"
-  "photoUrls": " " 
-  "tags": " "
-  "id_tag": "1 "
-  "name_tag": " "
-  "status": "available"
-}</t>
-  </si>
-  <si>
     <t>Agregar una nueva mascota, de manera exitosa solo con campos obligatorios.</t>
   </si>
   <si>
@@ -205,21 +196,6 @@
   </si>
   <si>
     <t>Agregar una nueva mascota capturando todos los campos.</t>
-  </si>
-  <si>
-    <t>1. Se debe mostrar status code 201.
-{
-  "id": 0,
-  "category": "gato",
-  "id_category": "1"
-  "name_category": "Bengala "
-  "name_mascota:": "Lucifer"
-  "photoUrls": "https://i.pinimg.com/originals/a2/cf/c4/a2cfc463c9e624185615b8eaca7d9aad.jpg." 
-  "tags": "Lu"
-  "id_tag": "1 "
-  "name_tag": "gato_bengala"
-  "status": "available"
-}</t>
   </si>
   <si>
     <t>Agregar una nueva mascota, dejando vacios los campos obligatorios.</t>
@@ -254,36 +230,7 @@
     <t>Actualizar informacion de una mascota</t>
   </si>
   <si>
-    <t>1. Se debe mostrar status code 200.
-{
-  "id": 0,
-  "category": "perro",
-  "id_category": "1"
-  "name_category": " "
-  "name_mascota:": "Loli"
-  "photoUrls": " " 
-  "tags": " "
-  "id_tag": "1 "
-  "name_tag": " "
-  "status": "available"
-}</t>
-  </si>
-  <si>
     <t>Validar que el identificador de mascota sea numero entero.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Seleccionar el metodo PUT.
-2. Teclear la URL: url /123/
-3. Capturar los siguientes campos obligatorios:
-- name: Loli
-- status: available
-- category: perro
-4. Dejar los demas campos vacios:
--name_category:" "
--photoUrls: " "
--name_tag: " "
-5. Dar clic en el boton SEND
-</t>
   </si>
   <si>
     <t>Actualizar informacion de una mascota, validar que permita actualizar y que el petId sea numero entero.</t>
@@ -293,22 +240,6 @@
   </si>
   <si>
     <t>CP11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Seleccionar el metodo PUT.
-2. Teclear la URL: url /#$23@/
-3. Capturar todos los campos:
--  "category": Perro
-- "id_category": "2"
-- "name_category": "12345 "
--  "name_mascota:": "12345"
--  "photoUrls": " " 
--  "tags": "pastor_Gail "
--  "id_tag": "2 "
--  "name_tag": "2-pastorGail"
--  "status": "available"
-4. Dar clic en el boton SEND
-</t>
   </si>
   <si>
     <t>1. Se debe mostrar status code 405.
@@ -330,14 +261,6 @@
     <t>Actualizar  una mascota en la tienda con datos de formulario.</t>
   </si>
   <si>
-    <t>1. Se debe mostrar status code 200.
-{
-  -URL: ulr/123
-  "name": "Galindo"
-  "status": "available"
-}</t>
-  </si>
-  <si>
     <t>Actualizar una mascota en la tienda con datos de formulario, validar que permita actualizar exitosamente.</t>
   </si>
   <si>
@@ -349,9 +272,6 @@
   <si>
     <t>1. Se debe mostrar status code 400
 Pet not found</t>
-  </si>
-  <si>
-    <t>Actualizar una mascota en la tienda con datos de formulario, validando el tipo de dato.</t>
   </si>
   <si>
     <t>1. Se debe mostrar status code 405
@@ -461,50 +381,6 @@
 1.- pet: 123
 2.- findByStatus: available
 4. Dar clic en el boton SEND
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Seleccionar el metodo POST.
-2. Teclear la URL: url /@#$/
-3. Capturar los siguientes campos:
--pet: @#$
-- name: 123
-- status: 123
-4. Dar clic en el boton SEND
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Seleccionar el metodo POST.
-2. Teclear la URL: url /@#$%/
-3. Capturar los siguientes campos:
--pet: @#$%
-- name: Galindo
-- status: available
-4. Dar clic en el boton SEND
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Seleccionar el metodo POST.
-2. Teclear la URL: url /123/
-3. Capturar los siguientes campos:
-- pet: 123
-- name: Galindo
-- status: available
-4. Dar clic en el boton SEND
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Seleccionar el metodo POST.
-2. Teclear la URL: url /pet/
-3. Capturar los siguientes campos:
-1.- category: gato
-2.- name_category: Bengala
-3.- name_mascota: Lucifer
-4.- photoUrls: https://i.pinimg.com/originals/a2/cf/c4/a2cfc463c9e624185615b8eaca7d9aad.jpg.
-5.- tags: Lu
-6.- name_tag: gato_bengala
-7.- status: available
-8. Dar clic en el boton SEND
 </t>
   </si>
   <si>
@@ -636,53 +512,10 @@
     <t>Agregar una nueva mascota capturando todos los campos y con status: pending.</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Seleccionar el metodo POST.
-2. Teclear la URL: url /pet/
-3. Capturar los siguientes campos:
-1.- category: gato
-2.- name_category: Bengala
-3.- name_mascota: Lucifer
-4.- photoUrls: https://i.pinimg.com/originals/a2/cf/c4/a2cfc463c9e624185615b8eaca7d9aad.jpg.
-5.- tags: Lu
-6.- name_tag: gato_bengala
-7.- status: pending
-8. Dar clic en el boton SEND
-</t>
-  </si>
-  <si>
-    <t>1. Se debe mostrar status code 201.
-{
-  "id": 0,
-  "category": "gato",
-  "id_category": "1"
-  "name_category": "Bengala "
-  "name_mascota:": "Lucifer"
-  "photoUrls": "https://i.pinimg.com/originals/a2/cf/c4/a2cfc463c9e624185615b8eaca7d9aad.jpg." 
-  "tags": "Lu"
-  "id_tag": "1 "
-  "name_tag": "gato_bengala"
-  "status": "pending"
-}</t>
-  </si>
-  <si>
     <t>Agregar una nueva mascota, de manera exitosa capturando todos los campos y status: solid.</t>
   </si>
   <si>
     <t>Agregar una nueva mascota capturando todos los campos y con status: solid.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Seleccionar el metodo POST.
-2. Teclear la URL: url /pet/
-3. Capturar los siguientes campos:
-1.- category: gato
-2.- name_category: Bengala
-3.- name_mascota: Lucifer
-4.- photoUrls: https://i.pinimg.com/originals/a2/cf/c4/a2cfc463c9e624185615b8eaca7d9aad.jpg.
-5.- tags: Lu
-6.- name_tag: gato_bengala
-7.- status: solid
-8. Dar clic en el boton SEND
-</t>
   </si>
   <si>
     <t>Agregar una nueva mascota, capturando los campos obligatorios con caracteres especiales.</t>
@@ -716,72 +549,10 @@
     <t>Actualizar informacion de una mascota exitosamente, validando la actualizacion capturando todos los campos y sea con status: pending.</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Seleccionar el metodo PUT.
-2. Teclear la URL: url /pet/
-3. Capturar todos los campos:
--  "category": Perro
-- "id_category": "2"
-- "name_category": "pastor "
--  "name_mascota:": "Gali"
--  "photoUrls": " " 
--  "tags": "pastor_Gail "
--  "id_tag": "2 "
--  "name_tag": "2-pastorGail"
--  "status": "pending"
-4. Dar clic en el boton SEND
-</t>
-  </si>
-  <si>
-    <t>1. Se debe mostrar status code 200.
-{
-  "id": 0,
-  "category": "perro",
-  "id_category": "2"
-  "name_category": "pastor"
-  "name_mascota:": "Gali"
-  "photoUrls": " " 
-  "tags": "pastor_Gali"
-  "id_tag": "2 "
-  "name_tag": "2-pastorGail "
-  "status": "pending"
-}</t>
-  </si>
-  <si>
     <t>Actualizar informacion de una mascota, validar que permita actualizar con status: solid.</t>
   </si>
   <si>
     <t>Actualizar informacion de una mascota exitosamente, validando la actualizacion capturando todos los campos y sea con status: solid.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Seleccionar el metodo PUT.
-2. Teclear la URL: url /pet/
-3. Capturar todos los campos:
--  "category": Perro
-- "id_category": "2"
-- "name_category": "pastor "
--  "name_mascota:": "Gali"
--  "photoUrls": " " 
--  "tags": "pastor_Gail "
--  "id_tag": "2 "
--  "name_tag": "2-pastorGail"
--  "status": "solid"
-4. Dar clic en el boton SEND
-</t>
-  </si>
-  <si>
-    <t>1. Se debe mostrar status code 200.
-{
-  "id": 0,
-  "category": "perro",
-  "id_category": "2"
-  "name_category": "pastor"
-  "name_mascota:": "Gali"
-  "photoUrls": " " 
-  "tags": "pastor_Gali"
-  "id_tag": "2 "
-  "name_tag": "2-pastorGail "
-  "status": "solid"
-}</t>
   </si>
   <si>
     <t>Actualizar informacion de una mascota, validar el PetId sea caracter especial.</t>
@@ -790,50 +561,10 @@
     <t>Actualizar informacion de una mascota, validando que el petId sea caracter especial.</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Seleccionar el metodo PUT.
-2. Teclear la URL: url /#$23@/
-3. Capturar todos los campos:
--  "category": Perro
-- "id_category": "2"
-- "id": @#$%
-- "name_category": "pastor "
--  "name_mascota:": "Gali"
--  "photoUrls": " " 
--  "tags": "pastor_Gail "
--  "id_tag": "2 "
--  "name_tag": "2-pastorGail"
--  "status": "available"
-4. Dar clic en el boton SEND
-</t>
-  </si>
-  <si>
-    <t>Actualizar informacion de una mascota, validando que el campo name sea String con longitud de 255 caracteres.</t>
-  </si>
-  <si>
-    <t>Actualizar informacion de una mascota, validar el campo name como String con longitud de 255 caracteres.</t>
-  </si>
-  <si>
     <t>Actualizar informacion de una mascota, validar el PetId este vacio.</t>
   </si>
   <si>
     <t>Actualizar informacion de una mascota, validando que el petId este vacio.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Seleccionar el metodo PUT.
-2. Teclear la URL: url /#$23@/
-3. Capturar todos los campos:
--  "category": Perro
-- "id_category": ""
-- "id":
-- "name_category": "pastor "
--  "name_mascota:": "Gali"
--  "photoUrls": " " 
--  "tags": "pastor_Gail "
--  "id_tag": " "
--  "name_tag": "2-pastorGail"
--  "status": "available"
-4. Dar clic en el boton SEND
-</t>
   </si>
   <si>
     <t>CP29</t>
@@ -891,6 +622,541 @@
   </si>
   <si>
     <t>Gherkin</t>
+  </si>
+  <si>
+    <t>Eliminar una mascota de la tienda por petId de manera exitosa con "petId" valor entero.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario: deletes a pet
+Given the path '/pet/{1}
+And Method DELETE
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario: deletes a pet
+Given the path '/pet/{12.22}
+And Method DELETE
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario: deletes a pet
+Given the path '/pet/{@#$}
+And Method DELETE
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario: deletes a pet
+Given the path '/pet/{  }
+And Method DELETE
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario: deletes a pet
+Given the path '/pet/{hola}
+And Method DELETE
+</t>
+  </si>
+  <si>
+    <t>Backgroud:
+*url=/pet/
+Scenario Outline: Add a pet with requiered fields.
+Given the path '/pet/
+And Method POST
+When the parameter are &lt;category&gt;&lt;status&gt; &lt;name&gt;
+Then status 200
+And match response
+{
+  "id": 1,
+  "category": {
+    "id": 01,
+    "name": "perro"
+  },
+  "name": "Loli",
+  "photoUrls": [
+    " "
+  ],
+  "tags": [
+    {
+      "id":01,
+      "name": ""
+    }
+  ],
+  "status": "available"
+}
+Examples:
+|id|name|category|status|
+|1|Loli|perro|available|
+|2|Lolo|gato|pending|
+|3|Lilis|canario|solid|</t>
+  </si>
+  <si>
+    <t>1. Se debe mostrar status code 201.
+{
+  "id": 1,
+***category***
+  "id_category": "1"
+  "name_category": "perro "
+  "name_mascota:": "Loli"
+  "photoUrls": " " 
+ **** "tags"*****
+  "id_tag": "1 "
+  "name_tag": " "
+  "status": "available"
+}</t>
+  </si>
+  <si>
+    <t>1. Se debe mostrar status code 201.
+{
+  "id": 22,
+  ***category****
+  "id_category": "22"
+  "name_category": "Bengala "
+******
+  "name_pet:": "Lucifer"
+  "photoUrls": "https://i.pinimg.com/originals/a2/cf/c4/a2cfc463c9e624185615b8eaca7d9aad.jpg." 
+****tags****
+    "id_tag": "22 "
+  "name_tag": "gato_bengala"
+  "status": "available"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar el metodo POST.
+2. Teclear la URL: url /pet/
+3. Capturar los siguientes campos:
+- id_category:22
+- name_category: Bengala
+- name_pet: Lucifer
+- photoUrls: https://i.pinimg.com/originals/a2/cf/c4/a2cfc463c9e624185615b8eaca7d9aad.jpg.
+- id_tag:22
+- name_tag: gato_bengala
+- status: available
+8. Dar clic en el boton SEND
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario: Add a pet with requiered fields empty
+Given the path '{{URL}}/pet/
+And Method POST
+When the parameter is name_pet = " " , name_category=" ", status=" "
+Then status code 405
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario: Add a pet with requiered fields name_pet, name_category, status with special caracters.
+Given the path '{{URL}}/pet/
+And Method POST
+When the parameter is name_pet = "@#% " , name_category="@#%", status="@#%"
+Then status code 405
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar el metodo POST.
+2. Teclear la URL: url /pet/
+3. Capturar los siguientes campos:
+- id_category:33
+- name_category: Michigan
+- name_pet: Luneta
+- photoUrls: https://i.pinimg.com/originals/a2/cf/c4/a2cfc463c9e624185615b8eaca7d9aad.jpg.
+- id_tag:33
+- name_tag: gato_michigan
+- status: pending
+8. Dar clic en el boton SEND
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar el metodo POST.
+2. Teclear la URL: url /pet/
+3. Capturar los siguientes campos:
+- id_category:44
+- name_category: Misifu
+- name_pet: Luna
+- photoUrls: https://i.pinimg.com/originals/a2/cf/c4/a2cfc463c9e624185615b8eaca7d9aad.jpg.
+- id_tag:44
+- name_tag: gato_misifu
+- status: solid
+8. Dar clic en el boton SEND
+</t>
+  </si>
+  <si>
+    <t>1. Se debe mostrar status code 201.
+{
+  "id": 44,
+  ***category****
+  "id_category": "44"
+  "name_category": "Misifu "
+******
+  "name_pet:": "Luna"
+  "photoUrls": "https://i.pinimg.com/originals/a2/cf/c4/a2cfc463c9e624185615b8eaca7d9aad.jpg." 
+****tags****
+    "id_tag": "44 "
+  "name_tag": "gato_misifu"
+  "status": "solid"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario Outline: Add a pet with all fields.
+Given the path '/pet/
+And Method POST
+When the parameter are &lt;id_category&gt; &lt;name_category&gt; &lt;name_pet&gt; &lt;photourls&gt; &lt;id_tag&gt; &lt;name_tag&gt; &lt;status&gt;
+Then status 200
+And match response
+{
+  "id": 22,
+  "category": {
+    "id": 22,
+    "name": "Bengala"
+  },
+  "name": "Lucifer",
+  "photoUrls": [
+    "photolucifer.jpg "
+  ],
+  "tags": [
+    {
+      "id":22,
+      "name": "gato_bengala"
+    }
+  ],
+  "status": "available"
+}
+Examples:
+|id_category|name_category|name_pet|photourl|id_tag|name_tag|status|
+|22|Bengala|Lucifer|photobengala|22|gato_bengala|available|
+|33Michigan|Luneta|photomichigan|33|gato_michigan|pending|
+|44|Misifu|Luna|photomisifu|44|gato_misifu|solid|
+</t>
+  </si>
+  <si>
+    <t>1. Se debe mostrar status code 201.
+{
+  "id": 22,
+  ***category****
+  "id_category": "33"
+  "name_category": "Michigan "
+******
+  "name_pet:": "Luneta"
+  "photoUrls": "https://i.pinimg.com/originals/a2/cf/c4/a2cfc463c9e624185615b8eaca7d9aad.jpg." 
+****tags****
+    "id_tag": "33 "
+  "name_tag": "gato_michigan"
+  "status": "pending"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar el metodo PUT.
+2. Teclear la URL: /pet/
+3. Capturar los siguientes campos obligatorios:
+- id_category:4
+- name_category: perro
+- name_pet: Ralu
+- status: available
+4. Dejar los demas campos vacios:
+-photoUrls: " "
+-id_tag: " "
+-name_tag: " "
+5. Dar clic en el boton SEND
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario: Update a pet with requiered fields.
+Given the path '/pet/
+And Method PUT
+When the parameter are &lt;id_category&gt; &lt;name_category&gt; &lt;name_pet&gt; &lt;status&gt; 
+Then status 200
+And match response
+{
+  "id": 4,
+  "category": {
+    "id": 4,
+    "name": "perro"
+  },
+  "name": "Ralu",
+  "photoUrls": [
+    " "
+  ],
+  "tags": [
+    {
+      "id":,
+      "name": ""
+    }
+  ],
+  "status": "available"
+}
+</t>
+  </si>
+  <si>
+    <t>1. Se debe mostrar status code 200.
+{
+  "id": 5,
+  "id_category": "5"
+  "name_category": "pastor"
+  "name_mascota:": "Gali"
+  "photoUrls": "photoGali" 
+  "id_tag": "5 "
+  "name_tag": "5-pastorGail "
+  "status": "pending"
+}</t>
+  </si>
+  <si>
+    <t>1. Se debe mostrar status code 200.
+{
+  "id": 4,
+  "id_category": "4"
+  "name_category": "perro"
+  "name_pet:": "Ralu"
+  "photoUrls": " " 
+  "id_tag": " "
+  "name_tag": " "
+  "status": "available"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar el metodo PUT.
+2. Teclear la URL: /pet/
+3. Capturar todos los campos:
+- "id_category": "5"
+- "name_category": "pastor "
+-  "name_pet:": "Gali"
+-  "photoUrls": "photoGali " 
+-  "id_tag": "5 "
+-  "name_tag": "5-pastorGail"
+-  "status": "solid"
+4. Dar clic en el boton SEND
+</t>
+  </si>
+  <si>
+    <t>Backgroud:
+*url=/pet/
+Scenario Outline: Update a pet with all fields, status pending and solid.
+Given the path '/pet/
+And Method PUT
+When the parameter are &lt;id_category&gt; &lt;name_category&gt; &lt;name_pet&gt; &lt;status&gt; 
+Then status 200
+And match response ==
+{
+  "id": 5,
+  "category": {
+    "id": 5,
+    "name": "pastor"
+  },
+  "name": "Gali",
+  "photoUrls": [
+    "photoGali"
+  ],
+  "tags": [
+    {
+      "id":5,
+      "name": "5-pastorGali"
+    }
+  ],
+  "status": "pending"
+}
+Examples:
+|id_category|name_category|name_pet|photoUrl|id_tag|name_tag|status|
+|5|pastor|Gali|photoGali|5|5-pastorGali|pending|
+|6|chihuahua|Goal|photoGoal|6|6-chihuahuaGoal|solid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar el metodo PUT.
+2. Teclear la URL: /pet/
+3. Capturar todos los campos:
+- "id_category": "6"
+- "name_category": "chihuahua "
+-  "name_pet:": "Goal"
+-  "photoUrls": "photoGoal " 
+-  "id_tag": "6 "
+-  "name_tag": "6-chihuahuaGoal"
+-  "status": "solid"
+4. Dar clic en el boton SEND
+</t>
+  </si>
+  <si>
+    <t>1. Se debe mostrar status code 200.
+{
+  "id": 5,
+  "id_category": "6"
+  "name_category": "chihuahua"
+  "name_pet:": "Goal"
+  "photoUrls": "photoGoal" 
+  "id_tag": "6"
+  "name_tag": "6-chihuahuaGoal"
+  "status": "solid"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar el metodo PUT.
+2. Teclear la URL: {url}/pet
+3. Capturar todos los campos:
+- "id": "2"
+- "id_category": @#$%
+- "name_category": "pastor "
+-  "name_pet": "Gali"
+-  "photoUrls": "photoGali " 
+-  "id_tag": "2 "
+-  "name_tag": "2-pastorGail"
+-  "status": "available"
+4. Dar clic en el boton SEND
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario: Update a pet with id fields special caracters.
+Given the path '{{URL}}/pet/
+And Method PUT
+When the parameter is id_category = "@#$%" 
+Then status code 405.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar el metodo PUT.
+2. Teclear la URL: {url}/pet
+3. Capturar todos los campos:
+- "id": "2"
+- "id_category": 
+- "name_category": "pastor "
+-  "name_pet": "Gali"
+-  "photoUrls": "photoGali " 
+-  "id_tag": "2 "
+-  "name_tag": "2-pastorGail"
+-  "status": "available"
+4. Dar clic en el boton SEND
+</t>
+  </si>
+  <si>
+    <t>Actualizar informacion de una mascota, validar el campo name pet como String con longitud de 255 caracteres.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar el metodo PUT.
+2. Teclear la URL: {url}/pet
+3. Capturar todos los campos:
+- "id": "2"
+- "id_category": 
+- "name_category": "pastor "
+-  "name_pet": "Gali1234567894561231452369874125369874523698541235"
+-  "photoUrls": "photoGali " 
+-  "id_tag": "2 "
+-  "name_tag": "2-pastorGail"
+-  "status": "available"
+4. Dar clic en el boton SEND
+</t>
+  </si>
+  <si>
+    <t>Actualizar informacion de una mascota, validando que el campo name sea String con longitud de 50 caracteres.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario: Update a pet with id pet fields is empty
+Given the path '{{URL}}/pet/
+And Method PUT
+When the parameter is id_category = " " 
+Then status code 405.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario: Update a pet with name_pet fields is 50 characters long.
+Given the path '{{URL}}/pet/
+And Method PUT
+When the parameter is id_pet = "Gali1234567894561231452369874125369874523698541235" 
+Then status code 405.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar el metodo POST.
+2. Teclear la URL: pet /{petId}/
+3. Capturar los siguientes campos:
+- petId: 123
+- name: Galindo
+- status: available
+4. Dar clic en el boton SEND
+</t>
+  </si>
+  <si>
+    <t>1. Se debe mostrar status code 200.
+{
+  -petId: 123
+  "name": "Galindo"
+  "status": "available"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario Outline: Update a pet with requiered fields.
+Given the path '/pet/
+And Method POST
+When the parameter are &lt;petId&gt; &lt;name&gt; &lt;status&gt; 
+Then status 200 
+Examples:
+|petId|name|status|
+|123|Galindo|available|
+|124|Galinde|available|
+|125|Galinda|available|
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar el metodo POST.
+2. Teclear la URL: pet /{petId}/
+3. Capturar los siguientes campos:
+- petId: @#$%
+- name: Galindo
+- status: available
+4. Dar clic en el boton SEND
+</t>
+  </si>
+  <si>
+    <t>Actualizar una mascota en la tienda con datos de formulario, validando petId vacio.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar el metodo POST.
+2. Teclear la URL: url /@#$/
+3. Capturar los siguientes campos:
+-petId:
+- name: 123
+- status: 123
+4. Dar clic en el boton SEND
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario: Update a pet with form petId is special characters.
+Given the path '/pet/
+And Method POST
+When the parameter are petId = @#$%
+Then status 400
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backgroud:
+*url=/pet/
+Scenario: Update a pet with form petId field is empty.
+Given the path '/pet/
+And Method POST
+When the parameter are &lt;petId&gt; &lt;name&gt; &lt;status&gt; 
+Then status 405
+</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1266,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1023,11 +1289,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1101,7 +1404,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1114,6 +1416,21 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1336,25 +1653,26 @@
   </sheetPr>
   <dimension ref="A1:AC1006"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView showGridLines="0" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.109375" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
     <col min="5" max="5" width="30.33203125" customWidth="1"/>
     <col min="6" max="6" width="33.33203125" customWidth="1"/>
-    <col min="7" max="7" width="37.109375" customWidth="1"/>
+    <col min="7" max="7" width="78.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="44.44140625" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" style="9"/>
     <col min="10" max="10" width="19" customWidth="1"/>
     <col min="11" max="11" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1385,13 +1703,13 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:29" ht="39.6" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>1</v>
@@ -1415,10 +1733,10 @@
         <v>7</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
@@ -1438,13 +1756,13 @@
       <c r="AB2" s="8"/>
       <c r="AC2" s="8"/>
     </row>
-    <row r="3" spans="1:29" s="15" customFormat="1" ht="277.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" s="15" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>22</v>
@@ -1453,7 +1771,7 @@
         <v>25</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>19</v>
@@ -1487,22 +1805,22 @@
       <c r="AB3" s="11"/>
       <c r="AC3" s="11"/>
     </row>
-    <row r="4" spans="1:29" s="20" customFormat="1" ht="277.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" s="20" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>26</v>
@@ -1534,13 +1852,13 @@
       <c r="AB4" s="16"/>
       <c r="AC4" s="16"/>
     </row>
-    <row r="5" spans="1:29" s="20" customFormat="1" ht="277.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" s="20" customFormat="1" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>33</v>
@@ -1549,7 +1867,7 @@
         <v>27</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>34</v>
@@ -1581,13 +1899,13 @@
       <c r="AB5" s="16"/>
       <c r="AC5" s="16"/>
     </row>
-    <row r="6" spans="1:29" s="20" customFormat="1" ht="277.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" s="20" customFormat="1" ht="158.4" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>29</v>
@@ -1596,7 +1914,7 @@
         <v>30</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>31</v>
@@ -1628,1319 +1946,813 @@
       <c r="AB6" s="16"/>
       <c r="AC6" s="16"/>
     </row>
-    <row r="7" spans="1:29" s="28" customFormat="1" ht="257.39999999999998" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="21"/>
-    </row>
-    <row r="8" spans="1:29" s="28" customFormat="1" ht="297" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="21"/>
-      <c r="AA8" s="21"/>
-      <c r="AB8" s="21"/>
-      <c r="AC8" s="21"/>
-    </row>
-    <row r="9" spans="1:29" s="28" customFormat="1" ht="297" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="21"/>
-      <c r="AC9" s="21"/>
-    </row>
-    <row r="10" spans="1:29" s="28" customFormat="1" ht="297" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="G10" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="H10" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="I10" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21"/>
-      <c r="AC10" s="21"/>
-    </row>
-    <row r="11" spans="1:29" s="27" customFormat="1" ht="178.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
-      <c r="X11" s="24"/>
-      <c r="Y11" s="24"/>
-      <c r="Z11" s="24"/>
-      <c r="AA11" s="24"/>
-      <c r="AB11" s="24"/>
-      <c r="AC11" s="24"/>
-    </row>
-    <row r="12" spans="1:29" s="27" customFormat="1" ht="178.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G12" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="H12" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-      <c r="X12" s="24"/>
-      <c r="Y12" s="24"/>
-      <c r="Z12" s="24"/>
-      <c r="AA12" s="24"/>
-      <c r="AB12" s="24"/>
-      <c r="AC12" s="24"/>
-    </row>
-    <row r="13" spans="1:29" s="29" customFormat="1" ht="257.39999999999998" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K13" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="11"/>
-      <c r="AB13" s="11"/>
-      <c r="AC13" s="11"/>
-    </row>
-    <row r="14" spans="1:29" s="29" customFormat="1" ht="277.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K14" s="32" t="s">
-        <v>158</v>
-      </c>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="11"/>
-      <c r="AB14" s="11"/>
-      <c r="AC14" s="11"/>
-    </row>
-    <row r="15" spans="1:29" s="29" customFormat="1" ht="277.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K15" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="11"/>
-      <c r="AC15" s="11"/>
-    </row>
-    <row r="16" spans="1:29" s="30" customFormat="1" ht="297" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K16" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="16"/>
-      <c r="V16" s="16"/>
-      <c r="W16" s="16"/>
-      <c r="X16" s="16"/>
-      <c r="Y16" s="16"/>
-      <c r="Z16" s="16"/>
-      <c r="AA16" s="16"/>
-      <c r="AB16" s="16"/>
-      <c r="AC16" s="16"/>
-    </row>
-    <row r="17" spans="1:29" s="30" customFormat="1" ht="297" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J17" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K17" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16"/>
-      <c r="V17" s="16"/>
-      <c r="W17" s="16"/>
-      <c r="X17" s="16"/>
-      <c r="Y17" s="16"/>
-      <c r="Z17" s="16"/>
-      <c r="AA17" s="16"/>
-      <c r="AB17" s="16"/>
-      <c r="AC17" s="16"/>
-    </row>
-    <row r="18" spans="1:29" s="30" customFormat="1" ht="277.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K18" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="16"/>
-      <c r="X18" s="16"/>
-      <c r="Y18" s="16"/>
-      <c r="Z18" s="16"/>
-      <c r="AA18" s="16"/>
-      <c r="AB18" s="16"/>
-      <c r="AC18" s="16"/>
-    </row>
-    <row r="19" spans="1:29" s="28" customFormat="1" ht="178.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="G19" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="H19" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K19" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
-      <c r="U19" s="21"/>
-      <c r="V19" s="21"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="21"/>
-      <c r="Y19" s="21"/>
-      <c r="Z19" s="21"/>
-      <c r="AA19" s="21"/>
-      <c r="AB19" s="21"/>
-      <c r="AC19" s="21"/>
-    </row>
-    <row r="20" spans="1:29" s="31" customFormat="1" ht="158.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="H20" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="I20" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="K20" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="24"/>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="24"/>
-      <c r="Z20" s="24"/>
-      <c r="AA20" s="24"/>
-      <c r="AB20" s="24"/>
-      <c r="AC20" s="24"/>
-    </row>
-    <row r="21" spans="1:29" s="31" customFormat="1" ht="158.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G21" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="H21" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="I21" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="K21" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="24"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
-      <c r="X21" s="24"/>
-      <c r="Y21" s="24"/>
-      <c r="Z21" s="24"/>
-      <c r="AA21" s="24"/>
-      <c r="AB21" s="24"/>
-      <c r="AC21" s="24"/>
-    </row>
-    <row r="22" spans="1:29" s="29" customFormat="1" ht="138.6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="11"/>
-      <c r="Y22" s="11"/>
-      <c r="Z22" s="11"/>
-      <c r="AA22" s="11"/>
-      <c r="AB22" s="11"/>
-      <c r="AC22" s="11"/>
-    </row>
-    <row r="23" spans="1:29" s="29" customFormat="1" ht="138.6" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
-      <c r="Y23" s="11"/>
-      <c r="Z23" s="11"/>
-      <c r="AA23" s="11"/>
-      <c r="AB23" s="11"/>
-      <c r="AC23" s="11"/>
-    </row>
-    <row r="24" spans="1:29" s="29" customFormat="1" ht="138.6" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="11"/>
-      <c r="AA24" s="11"/>
-      <c r="AB24" s="11"/>
-      <c r="AC24" s="11"/>
-    </row>
-    <row r="25" spans="1:29" s="30" customFormat="1" ht="138.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="I25" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J25" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="16"/>
-      <c r="S25" s="16"/>
-      <c r="T25" s="16"/>
-      <c r="U25" s="16"/>
-      <c r="V25" s="16"/>
-      <c r="W25" s="16"/>
-      <c r="X25" s="16"/>
-      <c r="Y25" s="16"/>
-      <c r="Z25" s="16"/>
-      <c r="AA25" s="16"/>
-      <c r="AB25" s="16"/>
-      <c r="AC25" s="16"/>
-    </row>
-    <row r="26" spans="1:29" s="28" customFormat="1" ht="158.4" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="H26" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="I26" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="J26" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
-      <c r="P26" s="21"/>
-      <c r="Q26" s="21"/>
-      <c r="R26" s="21"/>
-      <c r="S26" s="21"/>
-      <c r="T26" s="21"/>
-      <c r="U26" s="21"/>
-      <c r="V26" s="21"/>
-      <c r="W26" s="21"/>
-      <c r="X26" s="21"/>
-      <c r="Y26" s="21"/>
-      <c r="Z26" s="21"/>
-      <c r="AA26" s="21"/>
-      <c r="AB26" s="21"/>
-      <c r="AC26" s="21"/>
-    </row>
-    <row r="27" spans="1:29" s="31" customFormat="1" ht="138.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G27" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="H27" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="I27" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J27" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="24"/>
-      <c r="T27" s="24"/>
-      <c r="U27" s="24"/>
-      <c r="V27" s="24"/>
-      <c r="W27" s="24"/>
-      <c r="X27" s="24"/>
-      <c r="Y27" s="24"/>
-      <c r="Z27" s="24"/>
-      <c r="AA27" s="24"/>
-      <c r="AB27" s="24"/>
-      <c r="AC27" s="24"/>
-    </row>
-    <row r="28" spans="1:29" s="29" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="11"/>
-      <c r="T28" s="11"/>
-      <c r="U28" s="11"/>
-      <c r="V28" s="11"/>
-      <c r="W28" s="11"/>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="11"/>
-      <c r="Z28" s="11"/>
-      <c r="AA28" s="11"/>
-      <c r="AB28" s="11"/>
-      <c r="AC28" s="11"/>
-    </row>
-    <row r="29" spans="1:29" s="30" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="H29" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="I29" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K29" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16"/>
-      <c r="W29" s="16"/>
-      <c r="X29" s="16"/>
-      <c r="Y29" s="16"/>
-      <c r="Z29" s="16"/>
-      <c r="AA29" s="16"/>
-      <c r="AB29" s="16"/>
-      <c r="AC29" s="16"/>
-    </row>
-    <row r="30" spans="1:29" s="30" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="I30" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K30" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="16"/>
-      <c r="T30" s="16"/>
-      <c r="U30" s="16"/>
-      <c r="V30" s="16"/>
-      <c r="W30" s="16"/>
-      <c r="X30" s="16"/>
-      <c r="Y30" s="16"/>
-      <c r="Z30" s="16"/>
-      <c r="AA30" s="16"/>
-      <c r="AB30" s="16"/>
-      <c r="AC30" s="16"/>
-    </row>
-    <row r="31" spans="1:29" s="30" customFormat="1" ht="138.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="I31" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J31" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K31" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="L31" s="16"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16"/>
-      <c r="O31" s="16"/>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="16"/>
-      <c r="S31" s="16"/>
-      <c r="T31" s="16"/>
-      <c r="U31" s="16"/>
-      <c r="V31" s="16"/>
-      <c r="W31" s="16"/>
-      <c r="X31" s="16"/>
-      <c r="Y31" s="16"/>
-      <c r="Z31" s="16"/>
-      <c r="AA31" s="16"/>
-      <c r="AB31" s="16"/>
-      <c r="AC31" s="16"/>
-    </row>
-    <row r="32" spans="1:29" s="30" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="H32" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="I32" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J32" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K32" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="16"/>
-      <c r="T32" s="16"/>
-      <c r="U32" s="16"/>
-      <c r="V32" s="16"/>
-      <c r="W32" s="16"/>
-      <c r="X32" s="16"/>
-      <c r="Y32" s="16"/>
-      <c r="Z32" s="16"/>
-      <c r="AA32" s="16"/>
-      <c r="AB32" s="16"/>
-      <c r="AC32" s="16"/>
-    </row>
-    <row r="33" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+    </row>
+    <row r="8" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+    </row>
+    <row r="9" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+    </row>
+    <row r="10" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+    </row>
+    <row r="11" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+    </row>
+    <row r="12" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+    </row>
+    <row r="13" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+    </row>
+    <row r="14" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+    </row>
+    <row r="15" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+    </row>
+    <row r="16" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+    </row>
+    <row r="17" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+    </row>
+    <row r="18" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+    </row>
+    <row r="19" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+    </row>
+    <row r="20" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+    </row>
+    <row r="21" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+    </row>
+    <row r="22" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+    </row>
+    <row r="23" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+    </row>
+    <row r="24" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+    </row>
+    <row r="25" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+    </row>
+    <row r="26" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+    </row>
+    <row r="27" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+    </row>
+    <row r="28" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+    </row>
+    <row r="29" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+    </row>
+    <row r="30" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+    </row>
+    <row r="31" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+    </row>
+    <row r="32" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+    </row>
+    <row r="33" spans="1:29" ht="19.8" x14ac:dyDescent="0.7">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -33145,4 +32957,1662 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51683111-E537-4FF7-BCCD-90C8491C5BAD}">
+  <dimension ref="A2:AC6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="28" customFormat="1" ht="138.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+    </row>
+    <row r="4" spans="1:29" s="28" customFormat="1" ht="138.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+    </row>
+    <row r="5" spans="1:29" s="28" customFormat="1" ht="138.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+    </row>
+    <row r="6" spans="1:29" s="29" customFormat="1" ht="138.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J6" xr:uid="{E436D463-1F3D-444C-A87E-68B752DD07B6}">
+      <formula1>"PENDING,IN PROGRESS,BLOCKED,PASS,FAIL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0F2D60-EBBF-4109-86A8-348A2649ACF8}">
+  <dimension ref="A2:AC4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="27" customFormat="1" ht="158.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
+    </row>
+    <row r="4" spans="1:29" s="30" customFormat="1" ht="138.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="24"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J4" xr:uid="{CB88403D-479A-4FB6-AAD4-F7D3E75BB4B4}">
+      <formula1>"PENDING,IN PROGRESS,BLOCKED,PASS,FAIL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4663222F-34C7-42C8-B752-0178F5489DAB}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A2:AC8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="38.44140625" customWidth="1"/>
+    <col min="8" max="8" width="35" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="12" max="12" width="56.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="L4" s="34" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+      <c r="B5" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="L5" s="35"/>
+    </row>
+    <row r="6" spans="1:29" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="L6" s="36"/>
+    </row>
+    <row r="7" spans="1:29" ht="217.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="237.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L4:L6"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J8" xr:uid="{72CA316D-B365-4CE3-A822-32C7C7B83C71}">
+      <formula1>"PENDING,IN PROGRESS,BLOCKED,PASS,FAIL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA0CE4D-7E22-4878-BF3D-EF1E76A24D5D}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A2:AC8"/>
+  <sheetViews>
+    <sheetView topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" customWidth="1"/>
+    <col min="8" max="8" width="31.33203125" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.88671875" customWidth="1"/>
+    <col min="12" max="12" width="59.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="L4" s="37" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="257.39999999999998" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="L5" s="38"/>
+    </row>
+    <row r="6" spans="1:29" ht="257.39999999999998" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="257.39999999999998" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="297" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L4:L5"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J8" xr:uid="{BE3768DD-EAE5-4BAA-A6DA-66BDD918B049}">
+      <formula1>"PENDING,IN PROGRESS,BLOCKED,PASS,FAIL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FE1016-1310-49C7-B2E2-1CA4E74A3FFA}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A2:AC5"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="6" width="23.88671875" customWidth="1"/>
+    <col min="7" max="7" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="65.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="27" customFormat="1" ht="297" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
+    </row>
+    <row r="4" spans="1:29" s="30" customFormat="1" ht="198" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="24"/>
+    </row>
+    <row r="5" spans="1:29" s="30" customFormat="1" ht="198" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24"/>
+      <c r="Z5" s="24"/>
+      <c r="AA5" s="24"/>
+      <c r="AB5" s="24"/>
+      <c r="AC5" s="24"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J5" xr:uid="{D2191F90-47F8-4059-B9E0-6EA4CE56684A}">
+      <formula1>"PENDING,IN PROGRESS,BLOCKED,PASS,FAIL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5350A821-F434-476C-B788-5D3C7771083B}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A2:AC7"/>
+  <sheetViews>
+    <sheetView topLeftCell="G2" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.5546875" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+    </row>
+    <row r="3" spans="1:29" s="28" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+    </row>
+    <row r="4" spans="1:29" s="29" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="16"/>
+    </row>
+    <row r="5" spans="1:29" s="29" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+    </row>
+    <row r="6" spans="1:29" s="29" customFormat="1" ht="138.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+    </row>
+    <row r="7" spans="1:29" s="29" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J7" xr:uid="{687CC6FD-5D62-49AD-9EFE-FEA28CCE91C9}">
+      <formula1>"PENDING,IN PROGRESS,BLOCKED,PASS,FAIL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>